<commit_message>
Segunda carga de la segunda guia
</commit_message>
<xml_diff>
--- a/Clase3.xlsx
+++ b/Clase3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AlexRD\Laboratorio\Excel_Clase3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064A934A-569A-4F9D-AD80-9686FAE97896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C25C9E5-23F2-4A38-A177-9860E51FC0BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1CFF48EE-A392-4E1B-9CA1-AEA45C84C9F0}"/>
   </bookViews>
@@ -132,7 +132,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -145,6 +145,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -155,391 +165,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -934,11 +574,11 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:D6" ca="1" si="0">RANDBETWEEN(0,10)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">IF(AVERAGE(B2:D2)&gt;7,"PROMOCIONADO",IF(AVERAGE(B2:D2)&gt;3,"APROBADO","DESAPROBADO"))</f>
@@ -958,19 +598,19 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B6" ca="1" si="1">RANDBETWEEN(0,10)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E6" ca="1" si="2">IF(AVERAGE(B3:D3)&gt;7,"PROMOCIONADO",IF(AVERAGE(B3:D3)&gt;3,"APROBADO","DESAPROBADO"))</f>
-        <v>PROMOCIONADO</v>
+        <v>APROBADO</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F6" ca="1" si="3">IF(AND(AND(B3&gt;0,B3&lt;=10),AND(C3&gt;0,C3&lt;=10),AND(D3&gt;0,D3&lt;=10)),"OK","FALSO")</f>
@@ -990,11 +630,11 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1014,15 +654,15 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1039,15 +679,15 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1071,11 +711,15 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <f ca="1">IF(EXACT(A2,A9),AVERAGE(B2:D2),IF(EXACT(A3,A9),AVERAGE(B3:D3)))</f>
-        <v>4.333333333333333</v>
+        <v>8</v>
+      </c>
+      <c r="B9" t="b">
+        <f>IF(EXACT(A2,A9),AVERAGE(B2:D2),IF(EXACT(A3,A9),AVERAGE(B3:D3)))</f>
+        <v>0</v>
+      </c>
+      <c r="C9" t="str">
+        <f ca="1">VLOOKUP(A9,A2:F6,5,FALSE)</f>
+        <v>APROBADO</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1085,35 +729,35 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D6">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F6">
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="FALSO">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="FALSO">
       <formula>NOT(ISERROR(SEARCH("FALSO",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="DESAPROBADO">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="DESAPROBADO">
       <formula>NOT(ISERROR(SEARCH("DESAPROBADO",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="APROBADO">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="APROBADO">
       <formula>NOT(ISERROR(SEARCH("APROBADO",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PROMOCIONADO">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="PROMOCIONADO">
       <formula>NOT(ISERROR(SEARCH("PROMOCIONADO",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="DESAPROBADO">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="DESAPROBADO">
       <formula>NOT(ISERROR(SEARCH("DESAPROBADO",E2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ejercicio 2 en proceso
</commit_message>
<xml_diff>
--- a/Clase3.xlsx
+++ b/Clase3.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Estudios Superiores\ISNPT\Laboratorio\Excel\Guia_Nro2\GuiaNro2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB5FC2F-2909-4A65-802E-BC7F3CB54DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F513737B-D779-4667-860E-35EB6AA34B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{1CFF48EE-A392-4E1B-9CA1-AEA45C84C9F0}"/>
+    <workbookView xWindow="5115" yWindow="990" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{1CFF48EE-A392-4E1B-9CA1-AEA45C84C9F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejemplo" sheetId="1" r:id="rId1"/>
     <sheet name="Ejercicio1" sheetId="2" r:id="rId2"/>
+    <sheet name="Ejercicio2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ejercicio1!$A$1:$D$10</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Alumnos</t>
   </si>
@@ -176,13 +177,58 @@
   </si>
   <si>
     <t>Clase / Nota</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Long. Mano</t>
+  </si>
+  <si>
+    <t>Long. Pie</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>Ojos</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Azúl</t>
+  </si>
+  <si>
+    <t>Pelo</t>
+  </si>
+  <si>
+    <t>Rubio</t>
+  </si>
+  <si>
+    <t>Castaño</t>
+  </si>
+  <si>
+    <t>Calvo</t>
+  </si>
+  <si>
+    <t>Si Juan</t>
+  </si>
+  <si>
+    <t>Si Pablo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,16 +236,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -459,11 +527,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -485,12 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,6 +597,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,19 +1048,19 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,10)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:D6" ca="1" si="0">RANDBETWEEN(0,10)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">IF(AVERAGE(B2:D2)&gt;7,"PROMOCIONADO",IF(AVERAGE(B2:D2)&gt;3,"APROBADO","DESAPROBADO"))</f>
-        <v>APROBADO</v>
+        <v>DESAPROBADO</v>
       </c>
       <c r="F2" t="str">
         <f ca="1">IF(AND(AND(B2&gt;0,B2&lt;=10),AND(C2&gt;0,C2&lt;=10),AND(D2&gt;0,D2&lt;=10)),"OK","FALSO")</f>
@@ -977,23 +1076,23 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B6" ca="1" si="1">RANDBETWEEN(0,10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E6" ca="1" si="2">IF(AVERAGE(B3:D3)&gt;7,"PROMOCIONADO",IF(AVERAGE(B3:D3)&gt;3,"APROBADO","DESAPROBADO"))</f>
-        <v>DESAPROBADO</v>
+        <v>APROBADO</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F6" ca="1" si="3">IF(AND(AND(B3&gt;0,B3&lt;=10),AND(C3&gt;0,C3&lt;=10),AND(D3&gt;0,D3&lt;=10)),"OK","FALSO")</f>
-        <v>FALSO</v>
+        <v>OK</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -1005,7 +1104,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
@@ -1013,7 +1112,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1021,7 +1120,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>OK</v>
+        <v>FALSO</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -1033,19 +1132,19 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>PROMOCIONADO</v>
+        <v>APROBADO</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -1058,23 +1157,23 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>APROBADO</v>
+        <v>DESAPROBADO</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>FALSO</v>
+        <v>OK</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1148,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA492678-06C7-478F-8804-266E1BBE34FB}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -1173,10 +1272,10 @@
       <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1196,7 +1295,7 @@
       <c r="F2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="22" t="str">
+      <c r="G2" s="20" t="str">
         <f>"Clase: "&amp;(VLOOKUP(F2,A2:D10,2,FALSE))&amp;" - "&amp;"Nota: "&amp;(VLOOKUP(F2,A2:D10,4,FALSE))</f>
         <v>Clase: C - Nota: 5</v>
       </c>
@@ -1217,7 +1316,7 @@
       <c r="F3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="22" t="str">
+      <c r="G3" s="20" t="str">
         <f t="shared" ref="G3:G10" si="0">"Clase: "&amp;(VLOOKUP(F3,A3:D11,2,FALSE))&amp;" - "&amp;"Nota: "&amp;(VLOOKUP(F3,A3:D11,4,FALSE))</f>
         <v>Clase: A - Nota: 6</v>
       </c>
@@ -1238,7 +1337,7 @@
       <c r="F4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="22" t="str">
+      <c r="G4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: C - Nota: 6</v>
       </c>
@@ -1259,7 +1358,7 @@
       <c r="F5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="22" t="str">
+      <c r="G5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: A - Nota: 6,5</v>
       </c>
@@ -1280,7 +1379,7 @@
       <c r="F6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="22" t="str">
+      <c r="G6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: B - Nota: 7</v>
       </c>
@@ -1301,7 +1400,7 @@
       <c r="F7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="22" t="str">
+      <c r="G7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: B - Nota: 7,5</v>
       </c>
@@ -1322,7 +1421,7 @@
       <c r="F8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="22" t="str">
+      <c r="G8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: B - Nota: 8</v>
       </c>
@@ -1343,7 +1442,7 @@
       <c r="F9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="22" t="str">
+      <c r="G9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Clase: C - Nota: 8,5</v>
       </c>
@@ -1364,7 +1463,7 @@
       <c r="F10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="26" t="str">
+      <c r="G10" s="24" t="str">
         <f t="shared" si="0"/>
         <v>Clase: A - Nota: 9,5</v>
       </c>
@@ -1383,88 +1482,88 @@
       <c r="D12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="16">
         <f>AVERAGE(D2:D10)</f>
         <v>7.1111111111111107</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="17">
         <f>MAX(D2:D10)</f>
         <v>9.5</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="17">
         <f>MIN(D2:D10)</f>
         <v>5</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="18">
         <f>COUNTA(A2:A10)</f>
         <v>9</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="21" t="str">
+      <c r="J13" s="19" t="str">
         <f>VLOOKUP(A2,A2:D10,2,FALSE)&amp;"-"&amp;VLOOKUP(A2,A2:D10,4,FALSE)</f>
         <v>C-5</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="20">
         <f>COUNT(D6:D10)</f>
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23">
         <f>AVERAGE(D2:D10)</f>
         <v>7.1111111111111107</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="23">
         <f>AVERAGE(D3:D9)</f>
         <v>7.0714285714285712</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="23">
         <f>AVERAGE(D2:D6)</f>
         <v>6.1</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="23">
         <f>AVERAGE(D3:D8)</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="23">
         <f>AVERAGE(D4:D10)</f>
         <v>7.5714285714285712</v>
       </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1474,4 +1573,155 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653EBCC4-3A82-49CA-87DE-F471295D8662}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>187</v>
+      </c>
+      <c r="C2">
+        <v>167</v>
+      </c>
+      <c r="D2">
+        <v>198</v>
+      </c>
+      <c r="E2">
+        <f>IF(B2&gt;180,C2,D2)</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="31">
+        <v>30</v>
+      </c>
+      <c r="C3" s="18">
+        <v>56</v>
+      </c>
+      <c r="D3" s="18">
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <f>IF(D3&gt;B3,SUM(D3,B3,),AVERAGE(D3,B3))</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="31">
+        <v>35</v>
+      </c>
+      <c r="C4" s="18">
+        <v>40</v>
+      </c>
+      <c r="D4" s="18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="31">
+        <v>40</v>
+      </c>
+      <c r="C5" s="18">
+        <v>47</v>
+      </c>
+      <c r="D5" s="18">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="31">
+        <v>87</v>
+      </c>
+      <c r="C6" s="18">
+        <v>69</v>
+      </c>
+      <c r="D6" s="18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(B6&gt;C6,B7,C7)</f>
+        <v>Verde</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" t="str">
+        <f>IF(B8="Castaño","Castaño","Otro")</f>
+        <v>Otro</v>
+      </c>
+      <c r="F8" t="str">
+        <f>IF(OR(B8="Rubio",C8="Rubio"),"OK","NO OK")</f>
+        <v>OK</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>